<commit_message>
XF-965  AUTO_TC 6.2.2 Read overview layout of a Tenant -Check all labels in tenant overview section - Compare text from web elements method
Signed-off-by: Gerardo Soto <gerardo.soto@janeirodigital.com>
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
+++ b/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D660DF-FF2C-0547-8DA1-9ED6694E5D25}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E687C33-70D0-E046-A4D3-7CE57F6F1D10}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25220" windowHeight="12340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25220" windowHeight="12340" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Profiles" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="97">
   <si>
     <t>1</t>
   </si>
@@ -163,13 +163,172 @@
   </si>
   <si>
     <t>OropezaC</t>
+  </si>
+  <si>
+    <t>Title Name</t>
+  </si>
+  <si>
+    <t>Title Location</t>
+  </si>
+  <si>
+    <t>Title URL</t>
+  </si>
+  <si>
+    <t>Title Description</t>
+  </si>
+  <si>
+    <t>Title User</t>
+  </si>
+  <si>
+    <t>Title Quick Search</t>
+  </si>
+  <si>
+    <t>Tenant Name</t>
+  </si>
+  <si>
+    <t>Tenant Location</t>
+  </si>
+  <si>
+    <t>Tenant URL</t>
+  </si>
+  <si>
+    <t>Tenant Description</t>
+  </si>
+  <si>
+    <t>Find User</t>
+  </si>
+  <si>
+    <t>Tenant Management Title 1</t>
+  </si>
+  <si>
+    <t>Tenant Management Title 2</t>
+  </si>
+  <si>
+    <t>Tenant Management Title 3</t>
+  </si>
+  <si>
+    <t>Tenant Management Table Title 1</t>
+  </si>
+  <si>
+    <t>Tenant Management Table Title 2</t>
+  </si>
+  <si>
+    <t>Tenant Management Table Title 3</t>
+  </si>
+  <si>
+    <t>Tenant Management Table Title 4</t>
+  </si>
+  <si>
+    <t>Tenant Management Table Title 5</t>
+  </si>
+  <si>
+    <t>Tenant Creator Title</t>
+  </si>
+  <si>
+    <t>Web Site URL Title</t>
+  </si>
+  <si>
+    <t>No Of Tenants Title</t>
+  </si>
+  <si>
+    <t>No of roles title</t>
+  </si>
+  <si>
+    <t>Description Title</t>
+  </si>
+  <si>
+    <t>Tenant Location Title</t>
+  </si>
+  <si>
+    <t>Date Created Title</t>
+  </si>
+  <si>
+    <t>Overview Title</t>
+  </si>
+  <si>
+    <t>Tenant Name Title</t>
+  </si>
+  <si>
+    <t>Overview Table DescTitle</t>
+  </si>
+  <si>
+    <t>Overview Table User Title</t>
+  </si>
+  <si>
+    <t>Overview Table Date Title</t>
+  </si>
+  <si>
+    <t>QA tenant test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA Tenant Test </t>
+  </si>
+  <si>
+    <t>xform-stage.janeirodigital.com</t>
+  </si>
+  <si>
+    <t>This is an automation webdriver test</t>
+  </si>
+  <si>
+    <t>Gerardo Soto</t>
+  </si>
+  <si>
+    <t>Active Tenants</t>
+  </si>
+  <si>
+    <t>New Tenants in 30 days</t>
+  </si>
+  <si>
+    <t>New Users added</t>
+  </si>
+  <si>
+    <t>Tenant</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>No. of users</t>
+  </si>
+  <si>
+    <t>Tenant Administrators</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>Tenant Creator</t>
+  </si>
+  <si>
+    <t>Website Url</t>
+  </si>
+  <si>
+    <t>No. of tenants</t>
+  </si>
+  <si>
+    <t>No. of roles</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overview: </t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Date/Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +340,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -207,10 +374,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -771,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83198F83-9B0C-5E47-B8E1-F6AF02980682}">
   <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -810,12 +978,255 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA9D26B-0E60-8A47-AFEB-7FC72E92823D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:BL3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="1"/>
+      <c r="BC2" s="1"/>
+      <c r="BD2" s="1"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="1"/>
+      <c r="BJ2" s="1"/>
+      <c r="BK2" s="1"/>
+      <c r="BL2" s="1"/>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
XF-969 AUTO_TC 6.2.6 Read detailed info for a specific Role inside a Tenant - Read into a role
Signed-off-by: Gerardo Soto <gerardo.soto@janeirodigital.com>
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
+++ b/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E687C33-70D0-E046-A4D3-7CE57F6F1D10}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002A7B16-393D-CE4B-956F-1FD6CF09EBFC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25220" windowHeight="12340" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="1300" windowWidth="25220" windowHeight="12340" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Profiles" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="113">
   <si>
     <t>1</t>
   </si>
@@ -322,6 +322,54 @@
   </si>
   <si>
     <t>Date/Time</t>
+  </si>
+  <si>
+    <t>Company Logo Preview</t>
+  </si>
+  <si>
+    <t>Upload a file</t>
+  </si>
+  <si>
+    <t>Or</t>
+  </si>
+  <si>
+    <t>Color Preview</t>
+  </si>
+  <si>
+    <t>Navigation Bar</t>
+  </si>
+  <si>
+    <t>Subnavigation Bar</t>
+  </si>
+  <si>
+    <t>Navigation Links</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>Company Logo Preview Title</t>
+  </si>
+  <si>
+    <t>Upload a file Title</t>
+  </si>
+  <si>
+    <t>Or Title</t>
+  </si>
+  <si>
+    <t>Color Preview Title</t>
+  </si>
+  <si>
+    <t>Navigation Bar Title</t>
+  </si>
+  <si>
+    <t>Subnavigation Bar Title</t>
+  </si>
+  <si>
+    <t>Navigation Links Title</t>
+  </si>
+  <si>
+    <t>Background Title</t>
   </si>
 </sst>
 </file>
@@ -980,11 +1028,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA9D26B-0E60-8A47-AFEB-7FC72E92823D}">
   <dimension ref="A1:BL3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AJ8" sqref="AJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
@@ -1080,6 +1162,30 @@
       <c r="AF1" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="AG1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1178,14 +1284,30 @@
       <c r="AF2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
+      <c r="AG2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="AO2" s="1"/>
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
@@ -1236,7 +1358,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
XF-970 AUTO_TC 6.2.7 Read Users listed inside a Tenant - User listed read into a tenant
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
+++ b/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002A7B16-393D-CE4B-956F-1FD6CF09EBFC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B941162E-55F0-0846-8691-63726EF1DFFE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="1300" windowWidth="25220" windowHeight="12340" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="133">
   <si>
     <t>1</t>
   </si>
@@ -370,6 +370,66 @@
   </si>
   <si>
     <t>Background Title</t>
+  </si>
+  <si>
+    <t>FIRST NAME</t>
+  </si>
+  <si>
+    <t>LAST NAME</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>TENANT ADMINISTRATOR</t>
+  </si>
+  <si>
+    <t>INACTIVE</t>
+  </si>
+  <si>
+    <t>ACTIONS</t>
+  </si>
+  <si>
+    <t>FirstNameTitle</t>
+  </si>
+  <si>
+    <t>LastNameTitle</t>
+  </si>
+  <si>
+    <t>EmailTitle</t>
+  </si>
+  <si>
+    <t>TenantAdministratorTitle</t>
+  </si>
+  <si>
+    <t>InactiveTitle</t>
+  </si>
+  <si>
+    <t>ActionsTitle</t>
+  </si>
+  <si>
+    <t>Role Name</t>
+  </si>
+  <si>
+    <t>Role NameTitle</t>
+  </si>
+  <si>
+    <t>TimesAppliedTitle</t>
+  </si>
+  <si>
+    <t>Times Applied</t>
+  </si>
+  <si>
+    <t>LastEditTitle</t>
+  </si>
+  <si>
+    <t>Last Edit</t>
+  </si>
+  <si>
+    <t>sNoOfPermissionsTitle</t>
+  </si>
+  <si>
+    <t>no. of permissions</t>
   </si>
 </sst>
 </file>
@@ -1026,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA9D26B-0E60-8A47-AFEB-7FC72E92823D}">
-  <dimension ref="A1:BL3"/>
+  <dimension ref="A1:BP3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AJ8" sqref="AJ8"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AR5" sqref="AR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1066,9 +1126,10 @@
     <col min="38" max="38" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="17.5" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="14" bestFit="1" customWidth="1"/>
+    <col min="41" max="44" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:68" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>44</v>
       </c>
@@ -1186,8 +1247,38 @@
       <c r="AN1" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="AO1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AV1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AX1" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1308,16 +1399,36 @@
       <c r="AN2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1"/>
-      <c r="AU2" s="1"/>
-      <c r="AV2" s="1"/>
-      <c r="AW2" s="1"/>
-      <c r="AX2" s="1"/>
+      <c r="AO2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="AY2" s="1"/>
       <c r="AZ2" s="1"/>
       <c r="BA2" s="1"/>
@@ -1332,8 +1443,12 @@
       <c r="BJ2" s="1"/>
       <c r="BK2" s="1"/>
       <c r="BL2" s="1"/>
-    </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM2" s="1"/>
+      <c r="BN2" s="1"/>
+      <c r="BO2" s="1"/>
+      <c r="BP2" s="1"/>
+    </row>
+    <row r="3" spans="1:68" x14ac:dyDescent="0.2">
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1347,9 +1462,17 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="1"/>
+      <c r="AY3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
XF-972  AUTO_TC 6.3.1. Delete Tenants - Tenant Delete
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
+++ b/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B941162E-55F0-0846-8691-63726EF1DFFE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0907A67F-B296-1746-9C8A-9749BB583A47}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="1300" windowWidth="25220" windowHeight="12340" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="1300" windowWidth="25220" windowHeight="12340" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Profiles" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="135">
   <si>
     <t>1</t>
   </si>
@@ -430,6 +430,12 @@
   </si>
   <si>
     <t>no. of permissions</t>
+  </si>
+  <si>
+    <t>system@janeirodigital.com / ready2go</t>
+  </si>
+  <si>
+    <t>system@janeirodigital.com</t>
   </si>
 </sst>
 </file>
@@ -482,11 +488,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -938,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C742532F-29E1-8045-A2A4-412941127ACE}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -984,7 +991,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -995,13 +1002,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>30</v>
+      <c r="C5" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1012,7 +1019,7 @@
     <hyperlink ref="B3" r:id="rId4" xr:uid="{FD9E05EA-A4F9-144B-BAA8-53AB0E669186}"/>
     <hyperlink ref="C2" r:id="rId5" xr:uid="{59E2A097-E2DE-9647-81E8-36F2461D55C4}"/>
     <hyperlink ref="C4" r:id="rId6" xr:uid="{6E2CA544-906D-4A40-B931-96E3BBE61080}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{9F8A6EC4-B2A9-8245-9D1B-954A996D111A}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{B9080194-5440-3C49-A651-EA301588DF36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -1048,7 +1055,7 @@
   <dimension ref="A2:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1060,13 +1067,13 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
+      <c r="C2" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{5ACBBECA-2977-3545-A403-EEF5C50533DC}"/>
+    <hyperlink ref="C2" r:id="rId1" display="mailto:system@janeirodigital.com" xr:uid="{2BCD69C7-32D5-D047-A016-D7E36921790C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1088,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA9D26B-0E60-8A47-AFEB-7FC72E92823D}">
   <dimension ref="A1:BP3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="AR5" sqref="AR5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
XF-974 AUTO_TC 6.4.2 Update Tenant to Deactivated -Tenant Active or Deactivated
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
+++ b/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0907A67F-B296-1746-9C8A-9749BB583A47}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BB56C4-2559-1F45-8DA6-143EE5F97545}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="1300" windowWidth="25220" windowHeight="12340" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="1300" windowWidth="25220" windowHeight="12340" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Profiles" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="135">
   <si>
     <t>1</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Overview Table Date Title</t>
   </si>
   <si>
-    <t>QA tenant test</t>
-  </si>
-  <si>
     <t xml:space="preserve">QA Tenant Test </t>
   </si>
   <si>
@@ -432,10 +429,13 @@
     <t>no. of permissions</t>
   </si>
   <si>
-    <t>system@janeirodigital.com / ready2go</t>
-  </si>
-  <si>
     <t>system@janeirodigital.com</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>QA Tenant Test</t>
   </si>
 </sst>
 </file>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C742532F-29E1-8045-A2A4-412941127ACE}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1008,7 +1008,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1052,14 +1052,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83198F83-9B0C-5E47-B8E1-F6AF02980682}">
-  <dimension ref="A2:C2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
@@ -1068,14 +1076,15 @@
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="mailto:system@janeirodigital.com" xr:uid="{2BCD69C7-32D5-D047-A016-D7E36921790C}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{2BCD69C7-32D5-D047-A016-D7E36921790C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1095,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA9D26B-0E60-8A47-AFEB-7FC72E92823D}">
   <dimension ref="A1:BP3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AR5" sqref="AR5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1231,58 +1240,58 @@
         <v>74</v>
       </c>
       <c r="AG1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="AN1" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="AO1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AP1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="AP1" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="AQ1" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AR1" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AS1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AT1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="AX1" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:68" x14ac:dyDescent="0.2">
@@ -1307,134 +1316,134 @@
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="AA2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="AC2" s="1" t="s">
         <v>50</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AE2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AN2" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="AO2" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AS2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="AY2" s="1"/>
       <c r="AZ2" s="1"/>

</xml_diff>

<commit_message>
XF-977 AUTO_TC 6.4.5 Update Logo & Styles of Tenant - Positive - Change logo - Change background colors
Signed-off-by: Gerardo Soto <gerardo.soto@janeirodigital.com>
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
+++ b/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BB56C4-2559-1F45-8DA6-143EE5F97545}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5448A29-B227-E946-8822-3146FA5E1551}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="1300" windowWidth="25220" windowHeight="12340" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="139">
   <si>
     <t>1</t>
   </si>
@@ -436,6 +436,18 @@
   </si>
   <si>
     <t>QA Tenant Test</t>
+  </si>
+  <si>
+    <t>Logo Path</t>
+  </si>
+  <si>
+    <t>https://xform-stage.janeirodigital.com/assets/images/logo.png</t>
+  </si>
+  <si>
+    <t>BK Color</t>
+  </si>
+  <si>
+    <t>#04773f</t>
   </si>
 </sst>
 </file>
@@ -1104,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA9D26B-0E60-8A47-AFEB-7FC72E92823D}">
   <dimension ref="A1:BP3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AY7" sqref="AY7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1293,6 +1305,12 @@
       <c r="AX1" s="3" t="s">
         <v>123</v>
       </c>
+      <c r="AY1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AZ1" s="3" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="2" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1445,8 +1463,12 @@
       <c r="AX2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="AY2" s="1"/>
-      <c r="AZ2" s="1"/>
+      <c r="AY2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="BA2" s="1"/>
       <c r="BB2" s="1"/>
       <c r="BC2" s="1"/>

</xml_diff>

<commit_message>
XF-980 AUTO_TC 6.4.8 Roles - Create new Role -Create new role
Signed-off-by: Gerardo Soto <gerardo.soto@janeirodigital.com>
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
+++ b/xform-automation-webdriver/xform-controllers/src/main/resources/parameterFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5448A29-B227-E946-8822-3146FA5E1551}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9B8F4E-9AD3-0440-A5C1-E07D08D2B60D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="1300" windowWidth="25220" windowHeight="12340" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="142">
   <si>
     <t>1</t>
   </si>
@@ -448,6 +448,15 @@
   </si>
   <si>
     <t>#04773f</t>
+  </si>
+  <si>
+    <t>Role Permissions</t>
+  </si>
+  <si>
+    <t>Tenant Delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QATest Role </t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1126,7 @@
   <dimension ref="A1:BP3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AY7" sqref="AY7"/>
+      <selection activeCell="BC9" sqref="BC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1311,6 +1320,12 @@
       <c r="AZ1" s="3" t="s">
         <v>137</v>
       </c>
+      <c r="BA1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="BB1" s="3" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="2" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1469,8 +1484,12 @@
       <c r="AZ2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="BA2" s="1"/>
-      <c r="BB2" s="1"/>
+      <c r="BA2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="BC2" s="1"/>
       <c r="BD2" s="1"/>
       <c r="BE2" s="1"/>

</xml_diff>